<commit_message>
Added example grid to help me work through different scenarios
</commit_message>
<xml_diff>
--- a/test/support/start_cell_test_calculation_sheet.xlsx
+++ b/test/support/start_cell_test_calculation_sheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandbox\jake\fungus_toast\test\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2544D166-4875-40D5-B9E7-3A41863A9200}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0946C28E-4395-40EF-AC82-5312F50370E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{C6F7676B-7929-462B-A0BA-0C2172D2A12B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Start Cells" sheetId="1" r:id="rId1"/>
+    <sheet name="Example Grid" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Number of Rows and Columns</t>
   </si>
@@ -49,13 +50,24 @@
   <si>
     <t>Margin</t>
   </si>
+  <si>
+    <t>grid_size</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,7 +192,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:f>'Start Cells'!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -203,7 +216,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:f>'Start Cells'!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -496,7 +509,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$11</c:f>
+              <c:f>'Start Cells'!$D$7:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -520,7 +533,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$11</c:f>
+              <c:f>'Start Cells'!$E$7:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2454,4 +2467,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10BFBCDF-BDB8-4118-A431-5E627C147C36}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test file to illustrate aggregate calculations
</commit_message>
<xml_diff>
--- a/test/support/start_cell_test_calculation_sheet.xlsx
+++ b/test/support/start_cell_test_calculation_sheet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandbox\jake\fungus_toast\test\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0946C28E-4395-40EF-AC82-5312F50370E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AB4171-56EB-436B-B8D7-1CF8EC796A13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{C6F7676B-7929-462B-A0BA-0C2172D2A12B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" activeTab="2" xr2:uid="{C6F7676B-7929-462B-A0BA-0C2172D2A12B}"/>
   </bookViews>
   <sheets>
     <sheet name="Start Cells" sheetId="1" r:id="rId1"/>
     <sheet name="Example Grid" sheetId="2" r:id="rId2"/>
+    <sheet name="Example Aggregate Stats" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Number of Rows and Columns</t>
   </si>
@@ -53,12 +54,54 @@
   <si>
     <t>grid_size</t>
   </si>
+  <si>
+    <t>player_id</t>
+  </si>
+  <si>
+    <t>previous_player_id</t>
+  </si>
+  <si>
+    <t>live</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>Player 1 Live Cells</t>
+  </si>
+  <si>
+    <t>Player 1 Dead Cells</t>
+  </si>
+  <si>
+    <t>Player 1 Regenerated Cells</t>
+  </si>
+  <si>
+    <t>Player 2 Dead Cells</t>
+  </si>
+  <si>
+    <t>Player 2 Regenerated Cells</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Should not be possible. If the cell dies then the player id should move to previous player id</t>
+  </si>
+  <si>
+    <t>Should not be possible. If the cell is alive then the player_id should be set</t>
+  </si>
+  <si>
+    <t>Player 2 Live Cells</t>
+  </si>
+  <si>
+    <t>Should not be possible. If the cell is dead then there should be no player_id set</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +113,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,9 +145,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2237,7 +2288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9D3B51-EC0D-4E4A-AFD7-07FBE34F4866}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -2575,4 +2626,304 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63EF9FD-CEE5-43A9-8C38-97298138A99A}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>